<commit_message>
Results from n10 to n23
</commit_message>
<xml_diff>
--- a/py/tests/struct_sim_experiments/results/intra_n/n10/results_n_10.xlsx
+++ b/py/tests/struct_sim_experiments/results/intra_n/n10/results_n_10.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Comparisons intra level n = 10</t>
   </si>
@@ -28,7 +28,133 @@
     <t>n10_1 &lt;-&gt; n10_3</t>
   </si>
   <si>
+    <t>n10_1 &lt;-&gt; n10_4</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_5</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_6</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_1 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
     <t>n10_2 &lt;-&gt; n10_3</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_4</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_5</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_6</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_2 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_4</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_5</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_6</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_3 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_5</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_6</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_4 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_5 &lt;-&gt; n10_6</t>
+  </si>
+  <si>
+    <t>n10_5 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_5 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_5 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_5 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_6 &lt;-&gt; n10_7</t>
+  </si>
+  <si>
+    <t>n10_6 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_6 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_6 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_7 &lt;-&gt; n10_8</t>
+  </si>
+  <si>
+    <t>n10_7 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_7 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_8 &lt;-&gt; n10_9</t>
+  </si>
+  <si>
+    <t>n10_8 &lt;-&gt; n10_10</t>
+  </si>
+  <si>
+    <t>n10_9 &lt;-&gt; n10_10</t>
   </si>
   <si>
     <t>Average structural similarity between automatas created with parameter: 10</t>
@@ -363,7 +489,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -398,15 +524,351 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.6490436921296295</v>
+        <v>0.677637924382716</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>0.6834129050925926</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <f>AVERAGE(D5:D7)</f>
+        <v>0.7144820601851851</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>0.699941261574074</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0.6325276692708334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>0.5789930555555555</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>0.641384548611111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0.6490436921296295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>0.7345475260416667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>0.6697188464506173</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <v>0.701109905478395</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <v>0.7291999421296295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>0.6979754111207561</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <v>0.6711783854166665</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>0.6368301504629629</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <v>0.6297562210648148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>0.7026668595679012</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>0.7326725461355452</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>0.6478718171296295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <v>0.7775065104166666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <v>0.6847583912037037</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>0.7458887924382714</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <v>0.6309045862268517</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28">
+        <v>0.6576967592592592</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <v>0.700822120949074</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <v>0.6579499421296295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <v>0.6293995949074074</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <v>0.6264105902777779</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33">
+        <v>0.7090928819444443</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <v>0.6525169994212963</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35">
+        <v>0.6655092592592593</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36">
+        <v>0.6280729166666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <v>0.6895254629629629</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>0.6857024016203703</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <v>0.716525607638889</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40">
+        <v>0.6900327329282409</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="D41">
+        <v>0.7064465181327161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42">
+        <v>0.6363671875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>0.6027793451003086</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <v>0.6305164930555555</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <v>0.7296976273148149</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="D46">
+        <v>0.7613088348765432</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <v>0.6912871334876544</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <f>AVERAGE(D3:D47)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>